<commit_message>
Creación de gráficos según la proporción de empleados ausentes. Mejoras varias del código
</commit_message>
<xml_diff>
--- a/Planilla empleados total octubre 2024.xlsx
+++ b/Planilla empleados total octubre 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c82d1b869a3716e/Tecnicatura Cs datos e IA/2do cuatri/Practica I/Práctica San Jorge/Python San Jorge/Equipo_PP1-Clinica_San_Jorge-2C-2024-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_90296E556D9182E9E0C569813EFF590BB794DF8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEB32C0C-A2B3-44C0-8D2D-3DDC57B3E887}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_90296E556D9182E9E0C569813EFF590BB794DF8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F52336D1-04F0-43C0-A45B-9DCD2C902E70}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$4:$FU$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$4:$FU$412</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -3085,7 +3085,7 @@
   <dimension ref="A1:FU412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="35.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22915,11 +22915,6 @@
       <c r="FU412" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:FU4" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:FU412">
-      <sortCondition descending="1" ref="C4"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>